<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@c73d8f0f424432666ca8fc621efa5c7043023899 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -12,9 +12,9 @@
     <sheet name="Colors" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="1">'Costs'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="1">'Costs'!$H$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="1">'Costs'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="1">'Costs'!$H$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -26,7 +26,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0">
+    <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -87,12 +87,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Manufacturer of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Manufacturer number for each part and link to it's datasheet (Ctrl-click).
 Purple -&gt; Obsolete part detected by one of the distributors.</t>
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="G9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="H9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="136">
   <si>
     <t>Row</t>
   </si>
@@ -169,6 +182,36 @@
     <t>Datasheet</t>
   </si>
   <si>
+    <t>Specifications</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>JLCPCB ID</t>
+  </si>
+  <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>OC_FARNELL</t>
+  </si>
+  <si>
+    <t>OC_NEWARK</t>
+  </si>
+  <si>
+    <t>SUPPLIER</t>
+  </si>
+  <si>
+    <t>PACKAGE</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -184,7 +227,7 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>C_0504_1310Metric_Pad0.83x1.28mm_HandSolder</t>
+    <t>C_0805_2012Metric_Pad1.18x1.45mm_HandSolder</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -193,25 +236,76 @@
     <t>~</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>SMD Bipolar Electrolytic capacitor, Diameter 5.0mm, Heigth 5.4mm Alternate KiCad Library</t>
-  </si>
-  <si>
-    <t>C_Bipolar_SMD_D5.0mm_H5.4mm</t>
+    <t>0.22uF, Min 25V, 10%, X7R or similar</t>
+  </si>
+  <si>
+    <t>0.22uF_0603_25V</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>CGA3E2X5R1E224K080AA</t>
+  </si>
+  <si>
+    <t>0.22uF</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2.2uF, Min 25V 10% X5R</t>
+  </si>
+  <si>
+    <t>2.2uF_0603_25V</t>
   </si>
   <si>
     <t>C1</t>
   </si>
   <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>C_Elec_5x5.4</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>C_1206_3216Metric_Pad1.33x1.80mm_HandSolder</t>
+  </si>
+  <si>
+    <t>GRM188R6YA225KA12D</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>C57895</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>10uF, Min. 25V, X5R/X6S/X7R/X7S, 0805, MLCC</t>
+  </si>
+  <si>
+    <t>10uF_0805_25V</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM21BR61E106MA73-01.pdf</t>
+  </si>
+  <si>
+    <t>GRM21BR61E106MA73L</t>
+  </si>
+  <si>
+    <t>10uF/25V</t>
+  </si>
+  <si>
+    <t>C15850</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>Triple LED RVB (Avago Technology)</t>
@@ -232,9 +326,6 @@
     <t>https://media.digikey.com/pdf/Data%20Sheets/Harvatek%20PDFs/B3803FCH-20C001112U1930%20V1.3.pdf</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Generic connector, double row, 02x03, counter clockwise pin numbering scheme (similar to DIP package numbering), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -244,10 +335,31 @@
     <t>J1</t>
   </si>
   <si>
-    <t>PinHeader_2x03_P2.54mm_Vertical_SMD</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>PinSocket_2x03_P2.54mm_Vertical_SMD</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>IND_LQH32CN150K53L</t>
+  </si>
+  <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/P02/JELF243A-0030.pdf</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>SMD 0805 Chip Resistor, European Symbol, Alternate KiCad Library</t>
@@ -265,6 +377,42 @@
     <t>R_0603</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>3.4M</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>LT3494AEDDBPBF</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>DFN300X200X80-9N</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>46P5040</t>
+  </si>
+  <si>
+    <t>Linear Technology</t>
+  </si>
+  <si>
+    <t>DFN-8</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>3 Channel 12bit PWM constant currend LED Driver with single wire interface</t>
   </si>
   <si>
@@ -298,13 +446,10 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-22_19-36-40</t>
+    <t>2023-05-26_10-47-13</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -319,7 +464,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>11 (11 SMD/ 0 THT)</t>
+    <t>16 (16 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -334,6 +479,9 @@
     <t>Global Part Info</t>
   </si>
   <si>
+    <t>Manf</t>
+  </si>
+  <si>
     <t>Manf#</t>
   </si>
   <si>
@@ -346,6 +494,15 @@
     <t>Ext$</t>
   </si>
   <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>LT3494AEDDB#PBF</t>
+  </si>
+  <si>
     <t>Board Qty:</t>
   </si>
   <si>
@@ -358,7 +515,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-22 19:38:08</t>
+    <t>2023-05-26 10:48:39</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -807,7 +964,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>349959</xdr:colOff>
+      <xdr:colOff>16584</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1133,7 +1290,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1144,18 +1301,28 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="10" max="10" width="48.7109375" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" customHeight="1">
+    <row r="1" spans="1:19" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1163,78 +1330,88 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="F2" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:19">
       <c r="C6" s="2" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="F6" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1262,184 +1439,689 @@
       <c r="I8" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1">
+        <v>26</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="9" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="H10" s="9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1">
+        <v>27</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S10" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="I11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="30" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S12" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="30" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="45" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="J14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S14" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="30" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="45" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>45</v>
+      <c r="I15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="30" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S16" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="30" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S17" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q18" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="R18" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="30" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="R19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S19" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -1449,11 +2131,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <pane xSplit="8" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -1461,85 +2143,87 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="61.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" customHeight="1">
+    <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="13">
+        <v>93</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="15">
+        <v>95</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="16">
-        <f>SUM(G10:G15)</f>
+        <v>27</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="16">
+        <f>SUM(H10:H20)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -1547,8 +2231,9 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
@@ -1559,193 +2244,336 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>111</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="19" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="19">
+        <v>24</v>
+      </c>
+      <c r="F10" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G10" s="20">
-        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+      <c r="H10" s="20">
+        <f>IF(AND(ISNUMBER(F10),ISNUMBER(G10)),F10*G10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="19" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="19">
+        <v>24</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G11" s="20">
-        <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
+      <c r="H11" s="20">
+        <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1">
+    <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="19">
+        <v>114</v>
+      </c>
+      <c r="F12" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="20">
+        <f>IF(AND(ISNUMBER(F12),ISNUMBER(G12)),F12*G12,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" customHeight="1">
+      <c r="A13" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="20">
+        <f>IF(AND(ISNUMBER(F13),ISNUMBER(G13)),F13*G13,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" customHeight="1">
+      <c r="A14" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="19">
         <f>CEILING(BoardQty*6,1)</f>
         <v>6</v>
       </c>
-      <c r="G12" s="20">
-        <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
+      <c r="H14" s="20">
+        <f>IF(AND(ISNUMBER(F14),ISNUMBER(G14)),F14*G14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="19">
+    <row r="15" spans="1:8">
+      <c r="A15" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G13" s="20">
-        <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
+      <c r="H15" s="20">
+        <f>IF(AND(ISNUMBER(F15),ISNUMBER(G15)),F15*G15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="19">
+    <row r="16" spans="1:8" ht="30" customHeight="1">
+      <c r="A16" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G14" s="20">
-        <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
+      <c r="H16" s="20">
+        <f>IF(AND(ISNUMBER(F16),ISNUMBER(G16)),F16*G16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="19">
+    <row r="17" spans="1:8">
+      <c r="A17" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G15" s="20">
-        <f>IF(AND(ISNUMBER(E15),ISNUMBER(F15)),E15*F15,"")</f>
+      <c r="H17" s="20">
+        <f>IF(AND(ISNUMBER(F17),ISNUMBER(G17)),F17*G17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="23" t="s">
+    <row r="18" spans="1:8">
+      <c r="A18" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>73</v>
+      </c>
+      <c r="F18" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="20">
+        <f>IF(AND(ISNUMBER(F18),ISNUMBER(G18)),F18*G18,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="20">
+        <f>IF(AND(ISNUMBER(F19),ISNUMBER(G19)),F19*G19,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="20">
+        <f>IF(AND(ISNUMBER(F20),ISNUMBER(G20)),F20*G20,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="23" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="D1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="F10">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(ISBLANK(D10),TRUE())</formula>
+      <formula>AND(ISBLANK(E10),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="F11">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(ISBLANK(D11),TRUE())</formula>
+      <formula>AND(ISBLANK(E11),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND(ISBLANK(D12),TRUE())</formula>
+      <formula>AND(ISBLANK(E12),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
+  <conditionalFormatting sqref="F13">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>AND(ISBLANK(D13),TRUE())</formula>
+      <formula>AND(ISBLANK(E13),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
+  <conditionalFormatting sqref="F14">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>AND(ISBLANK(D14),TRUE())</formula>
+      <formula>AND(ISBLANK(E14),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+  <conditionalFormatting sqref="F15">
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>AND(ISBLANK(D15),TRUE())</formula>
+      <formula>AND(ISBLANK(E15),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>AND(ISBLANK(E16),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>AND(ISBLANK(E17),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>AND(ISBLANK(E18),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="expression" dxfId="0" priority="10">
+      <formula>AND(ISBLANK(E19),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="expression" dxfId="0" priority="11">
+      <formula>AND(ISBLANK(E20),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1"/>
-    <hyperlink ref="D15" r:id="rId2"/>
+    <hyperlink ref="E13" r:id="rId1"/>
+    <hyperlink ref="E14" r:id="rId2"/>
+    <hyperlink ref="E16" r:id="rId3"/>
+    <hyperlink ref="E20" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1762,72 +2590,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@1d9ed117c9126df0080f8c39c33eaa05274bdab9 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -449,7 +449,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_10-47-13</t>
+    <t>2023-05-26_11-18-00</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -515,7 +515,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 10:48:39</t>
+    <t>2023-05-26 11:20:01</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@b588e1f38028e9f3b1bf420905f7dcc9f6fbcaa8 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -449,7 +449,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_11-18-00</t>
+    <t>2023-05-26_11-30-56</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -515,7 +515,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 11:20:01</t>
+    <t>2023-05-26 11:33:02</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@a9522a1134bc8fcc3357c5b1b8ef2f5621952c79 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -449,7 +449,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_11-30-56</t>
+    <t>2023-05-26_12-41-36</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -515,7 +515,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 11:33:02</t>
+    <t>2023-05-26 12:43:07</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@ead96919bd932af91e7ff376295529b0450fa5f4 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -449,7 +449,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_12-41-36</t>
+    <t>2023-05-26_12-47-20</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -515,7 +515,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 12:43:07</t>
+    <t>2023-05-26 12:48:56</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@9c937b27a9d8118f423216fad60acce93a302887 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -449,7 +449,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_12-47-20</t>
+    <t>2023-05-26_13-10-25</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -515,7 +515,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 12:48:56</t>
+    <t>2023-05-26 13:11:55</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@cba3eb4054242e81c05ac62920c6e6053809142d 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -449,7 +449,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_13-10-25</t>
+    <t>2023-05-26_13-43-58</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -515,7 +515,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 13:11:55</t>
+    <t>2023-05-26 13:45:29</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@84089f471b9e7f6a596906c797a877477eed6009 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="149">
   <si>
     <t>Row</t>
   </si>
@@ -197,6 +197,9 @@
     <t>JLCPCB ID</t>
   </si>
   <si>
+    <t>SUPPLIER</t>
+  </si>
+  <si>
     <t>MPN</t>
   </si>
   <si>
@@ -206,9 +209,6 @@
     <t>OC_NEWARK</t>
   </si>
   <si>
-    <t>SUPPLIER</t>
-  </si>
-  <si>
     <t>PACKAGE</t>
   </si>
   <si>
@@ -224,7 +224,7 @@
     <t>C2</t>
   </si>
   <si>
-    <t>100nF</t>
+    <t>330nF</t>
   </si>
   <si>
     <t>C_0805_2012Metric_Pad1.18x1.45mm_HandSolder</t>
@@ -233,12 +233,15 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>~</t>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM216R61A334KA01-01.pdf</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/GRM216R61A334KA01D/2545090</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -272,6 +275,9 @@
     <t>C_1206_3216Metric_Pad1.33x1.80mm_HandSolder</t>
   </si>
   <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRT31CR61H225KE01-01.pdf</t>
+  </si>
+  <si>
     <t>GRM188R6YA225KA12D</t>
   </si>
   <si>
@@ -281,6 +287,9 @@
     <t>C57895</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/GRT31CR61H225KE01L/5416882</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
@@ -293,7 +302,7 @@
     <t>C3</t>
   </si>
   <si>
-    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM21BR61E106MA73-01.pdf</t>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRT31CR6YA106KE01-01.pdf</t>
   </si>
   <si>
     <t>GRM21BR61E106MA73L</t>
@@ -305,6 +314,9 @@
     <t>C15850</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/GRT31CR6YA106KE01K/13904946</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
@@ -326,6 +338,9 @@
     <t>https://media.digikey.com/pdf/Data%20Sheets/Harvatek%20PDFs/B3803FCH-20C001112U1930%20V1.3.pdf</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/harvatek-corporation/B3803FCH-20C001112U1930/13588742</t>
+  </si>
+  <si>
     <t>Generic connector, double row, 02x03, counter clockwise pin numbering scheme (similar to DIP package numbering), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -338,6 +353,12 @@
     <t>PinSocket_2x03_P2.54mm_Vertical_SMD</t>
   </si>
   <si>
+    <t>https://www.precidip.com/AppHost/9696,1/Scripts/Modules/Catalog/Default.aspx?c=7&amp;i=349&amp;p=124&amp;pdf=1&amp;dsku=853-PP-NNN-30-001101</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/preci-dip/853-87-006-30-001101/4137372</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
@@ -359,6 +380,9 @@
     <t>https://search.murata.co.jp/Ceramy/image/img/P02/JELF243A-0030.pdf</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/LQH32CN150K53L/1016219</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
@@ -377,6 +401,12 @@
     <t>R_0603</t>
   </si>
   <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Samsung%20PDFs/RC_Series_ds.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/RC1608F512CS/3965020</t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
@@ -386,6 +416,9 @@
     <t>3.4M</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/RC1608F3484CS/3965270</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
@@ -398,15 +431,18 @@
     <t>DFN300X200X80-9N</t>
   </si>
   <si>
+    <t>https://www.analog.com/media/en/technical-documentation/data-sheets/3494fb.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/analog-devices-inc/LT3494AEDDB-TRPBF/1767840</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
     <t>46P5040</t>
   </si>
   <si>
-    <t>Linear Technology</t>
-  </si>
-  <si>
     <t>DFN-8</t>
   </si>
   <si>
@@ -425,7 +461,10 @@
     <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
-    <t>http://www.ti.com/lit/ds/symlink/tlc5973.pdf</t>
+    <t>https://www.ti.com/lit/ds/symlink/tlc5973.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/texas-instruments/TLC5973DR/4251271</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -449,7 +488,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_13-43-58</t>
+    <t>2023-05-26_14-20-59</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -515,7 +554,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 13:45:29</t>
+    <t>2023-05-26 14:22:42</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -964,7 +1003,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>16584</xdr:colOff>
+      <xdr:colOff>83259</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1303,7 +1342,7 @@
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
@@ -1313,16 +1352,16 @@
     <col min="12" max="12" width="25.7109375" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
     <col min="14" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.7109375" customWidth="1"/>
-    <col min="18" max="18" width="22.7109375" customWidth="1"/>
+    <col min="15" max="15" width="60.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" customWidth="1"/>
     <col min="19" max="19" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1343,13 +1382,13 @@
     </row>
     <row r="2" spans="1:19">
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="F2" s="3">
         <v>11</v>
@@ -1357,41 +1396,41 @@
     </row>
     <row r="3" spans="1:19">
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="C4" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="C5" s="2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1399,13 +1438,13 @@
     </row>
     <row r="6" spans="1:19">
       <c r="C6" s="2" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="F6" s="3">
         <v>16</v>
@@ -1470,7 +1509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -1495,7 +1534,7 @@
       <c r="H9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="J9" s="8" t="s">
@@ -1513,8 +1552,8 @@
       <c r="N9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="8" t="s">
-        <v>27</v>
+      <c r="O9" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>27</v>
@@ -1529,21 +1568,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" ht="30" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>24</v>
@@ -1554,26 +1593,26 @@
       <c r="H10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>27</v>
+      <c r="I10" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>27</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="12" t="s">
-        <v>27</v>
+      <c r="O10" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="P10" s="12" t="s">
         <v>27</v>
@@ -1588,24 +1627,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>19</v>
@@ -1613,26 +1652,26 @@
       <c r="H11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>27</v>
+      <c r="I11" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>27</v>
+        <v>43</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>27</v>
@@ -1649,22 +1688,22 @@
     </row>
     <row r="12" spans="1:19" ht="30" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>19</v>
@@ -1673,25 +1712,25 @@
         <v>25</v>
       </c>
       <c r="I12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="K12" s="12" t="s">
         <v>27</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>27</v>
+        <v>52</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="P12" s="12" t="s">
         <v>27</v>
@@ -1708,31 +1747,31 @@
     </row>
     <row r="13" spans="1:19" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>27</v>
@@ -1749,8 +1788,8 @@
       <c r="N13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O13" s="8" t="s">
-        <v>27</v>
+      <c r="O13" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="P13" s="8" t="s">
         <v>27</v>
@@ -1767,22 +1806,22 @@
     </row>
     <row r="14" spans="1:19" ht="45" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>19</v>
@@ -1790,8 +1829,8 @@
       <c r="H14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>26</v>
+      <c r="I14" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>27</v>
@@ -1808,8 +1847,8 @@
       <c r="N14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="12" t="s">
-        <v>27</v>
+      <c r="O14" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="P14" s="12" t="s">
         <v>27</v>
@@ -1826,22 +1865,22 @@
     </row>
     <row r="15" spans="1:19" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>19</v>
@@ -1850,7 +1889,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>27</v>
@@ -1867,8 +1906,8 @@
       <c r="N15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O15" s="8" t="s">
-        <v>27</v>
+      <c r="O15" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="P15" s="8" t="s">
         <v>27</v>
@@ -1885,22 +1924,22 @@
     </row>
     <row r="16" spans="1:19" ht="30" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>19</v>
@@ -1908,8 +1947,8 @@
       <c r="H16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="12" t="s">
-        <v>26</v>
+      <c r="I16" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>27</v>
@@ -1926,8 +1965,8 @@
       <c r="N16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="12" t="s">
-        <v>27</v>
+      <c r="O16" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="P16" s="12" t="s">
         <v>27</v>
@@ -1944,22 +1983,22 @@
     </row>
     <row r="17" spans="1:19" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>19</v>
@@ -1967,8 +2006,8 @@
       <c r="H17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>26</v>
+      <c r="I17" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>27</v>
@@ -1985,8 +2024,8 @@
       <c r="N17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="8" t="s">
-        <v>27</v>
+      <c r="O17" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="P17" s="8" t="s">
         <v>27</v>
@@ -2001,24 +2040,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" ht="30" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>19</v>
@@ -2026,8 +2065,8 @@
       <c r="H18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="12" t="s">
-        <v>27</v>
+      <c r="I18" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="J18" s="12" t="s">
         <v>27</v>
@@ -2044,40 +2083,40 @@
       <c r="N18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="O18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" s="10" t="s">
-        <v>81</v>
+      <c r="O18" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="R18" s="10" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>19</v>
@@ -2086,7 +2125,7 @@
         <v>25</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>27</v>
@@ -2103,8 +2142,8 @@
       <c r="N19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O19" s="8" t="s">
-        <v>27</v>
+      <c r="O19" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>27</v>
@@ -2143,7 +2182,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="16.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="61.7109375" customWidth="1" outlineLevel="1"/>
@@ -2154,7 +2193,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2163,13 +2202,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -2177,13 +2216,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2192,13 +2231,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H20)</f>
@@ -2207,23 +2246,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2244,22 +2283,22 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>22</v>
       </c>
@@ -2268,6 +2307,9 @@
       </c>
       <c r="C10" s="19" t="s">
         <v>24</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>26</v>
       </c>
       <c r="F10" s="19">
         <f>BoardQty*1</f>
@@ -2278,18 +2320,21 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="30" customHeight="1">
       <c r="A11" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>113</v>
+        <v>126</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>26</v>
       </c>
       <c r="F11" s="19">
         <f>BoardQty*1</f>
@@ -2300,18 +2345,21 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>36</v>
-      </c>
       <c r="C12" s="19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>114</v>
+        <v>127</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="F12" s="19">
         <f>BoardQty*1</f>
@@ -2324,19 +2372,19 @@
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F13" s="19">
         <f>BoardQty*1</f>
@@ -2349,16 +2397,16 @@
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F14" s="19">
         <f>CEILING(BoardQty*6,1)</f>
@@ -2369,15 +2417,18 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="45" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="F15" s="19">
         <f>BoardQty*1</f>
@@ -2390,16 +2441,16 @@
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F16" s="19">
         <f>BoardQty*1</f>
@@ -2410,15 +2461,18 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="30" customHeight="1">
       <c r="A17" s="19" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>73</v>
+        <v>81</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="F17" s="19">
         <f>BoardQty*1</f>
@@ -2429,15 +2483,18 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="30" customHeight="1">
       <c r="A18" s="19" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>73</v>
+        <v>81</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="F18" s="19">
         <f>BoardQty*1</f>
@@ -2450,16 +2507,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="F19" s="19">
         <f>BoardQty*1</f>
@@ -2472,16 +2529,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="F20" s="19">
         <f>BoardQty*1</f>
@@ -2494,15 +2551,15 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="21" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="23" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2566,14 +2623,21 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1"/>
-    <hyperlink ref="E14" r:id="rId2"/>
-    <hyperlink ref="E16" r:id="rId3"/>
-    <hyperlink ref="E20" r:id="rId4"/>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E11" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="E13" r:id="rId4"/>
+    <hyperlink ref="E14" r:id="rId5"/>
+    <hyperlink ref="E15" r:id="rId6"/>
+    <hyperlink ref="E16" r:id="rId7"/>
+    <hyperlink ref="E17" r:id="rId8"/>
+    <hyperlink ref="E18" r:id="rId9"/>
+    <hyperlink ref="E19" r:id="rId10"/>
+    <hyperlink ref="E20" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <drawing r:id="rId12"/>
+  <legacyDrawing r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -2590,72 +2654,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@7884b48234a3ceb3c8726289c09fb48f6e2db824 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -488,7 +488,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_14-20-59</t>
+    <t>2023-05-26_14-22-24</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -554,7 +554,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 14:22:42</t>
+    <t>2023-05-26 14:24:12</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@1700bd16053fd4b3e2c698d5dc94816918e5af73 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="149">
   <si>
     <t>Row</t>
   </si>
@@ -353,7 +353,7 @@
     <t>PinSocket_2x03_P2.54mm_Vertical_SMD</t>
   </si>
   <si>
-    <t>https://www.precidip.com/AppHost/9696,1/Scripts/Modules/Catalog/Default.aspx?c=7&amp;i=349&amp;p=124&amp;pdf=1&amp;dsku=853-PP-NNN-30-001101</t>
+    <t>~</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/preci-dip/853-87-006-30-001101/4137372</t>
@@ -428,7 +428,7 @@
     <t>U2</t>
   </si>
   <si>
-    <t>DFN300X200X80-9N</t>
+    <t>DFN-8-1EP_2x3mm_P0.5mm_EP0.61x2.2mm</t>
   </si>
   <si>
     <t>https://www.analog.com/media/en/technical-documentation/data-sheets/3494fb.pdf</t>
@@ -488,7 +488,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_14-22-24</t>
+    <t>2023-05-26_17-21-17</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -554,7 +554,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 14:24:12</t>
+    <t>2023-05-26 17:22:47</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -1829,7 +1829,7 @@
       <c r="H14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="12" t="s">
         <v>66</v>
       </c>
       <c r="J14" s="12" t="s">
@@ -2417,7 +2417,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45" customHeight="1">
+    <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
         <v>64</v>
       </c>
@@ -2426,9 +2426,6 @@
       </c>
       <c r="C15" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>66</v>
       </c>
       <c r="F15" s="19">
         <f>BoardQty*1</f>
@@ -2628,16 +2625,15 @@
     <hyperlink ref="E12" r:id="rId3"/>
     <hyperlink ref="E13" r:id="rId4"/>
     <hyperlink ref="E14" r:id="rId5"/>
-    <hyperlink ref="E15" r:id="rId6"/>
-    <hyperlink ref="E16" r:id="rId7"/>
-    <hyperlink ref="E17" r:id="rId8"/>
-    <hyperlink ref="E18" r:id="rId9"/>
-    <hyperlink ref="E19" r:id="rId10"/>
-    <hyperlink ref="E20" r:id="rId11"/>
+    <hyperlink ref="E16" r:id="rId6"/>
+    <hyperlink ref="E17" r:id="rId7"/>
+    <hyperlink ref="E18" r:id="rId8"/>
+    <hyperlink ref="E19" r:id="rId9"/>
+    <hyperlink ref="E20" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId12"/>
-  <legacyDrawing r:id="rId13"/>
+  <drawing r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@53e1939828b68477ddfdde2ee1498c577922519b 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -488,7 +488,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_17-21-17</t>
+    <t>2023-05-26_17-26-11</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -554,7 +554,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 17:22:47</t>
+    <t>2023-05-26 17:27:38</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@23f57f1a93c667ae5fe27b4edf27bde85dcf633c 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -488,7 +488,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-26_17-26-11</t>
+    <t>2023-05-28_08-21-26</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -554,7 +554,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-26 17:27:38</t>
+    <t>2023-05-28 08:23:20</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@3e57fad6be272f79afc6395a4ce0ade73bc728c0 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="150">
   <si>
     <t>Row</t>
   </si>
@@ -485,10 +485,13 @@
     <t>Revision:</t>
   </si>
   <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-05-28_08-21-26</t>
+    <t>2023-05-29</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -554,7 +557,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-28 08:23:20</t>
+    <t>2023-05-29 10:57:25</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -1388,7 +1391,7 @@
         <v>106</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F2" s="3">
         <v>11</v>
@@ -1402,10 +1405,10 @@
         <v>108</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1413,24 +1416,24 @@
         <v>109</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="C5" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1438,13 +1441,13 @@
     </row>
     <row r="6" spans="1:19">
       <c r="C6" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F6" s="3">
         <v>16</v>
@@ -2208,7 +2211,7 @@
         <v>106</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -2222,7 +2225,7 @@
         <v>108</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2234,10 +2237,10 @@
         <v>109</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H20)</f>
@@ -2246,23 +2249,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2283,19 +2286,19 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1">
@@ -2331,7 +2334,7 @@
         <v>24</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>26</v>
@@ -2356,7 +2359,7 @@
         <v>39</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>40</v>
@@ -2381,7 +2384,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>49</v>
@@ -2513,7 +2516,7 @@
         <v>91</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F19" s="19">
         <f>BoardQty*1</f>
@@ -2548,15 +2551,15 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2650,72 +2653,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@28e6f07c7e069da3a8f82a83f37badbbd11a2b68 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -211,7 +211,7 @@
     <t>LED_SK6812_EC15_1.5x1.5mm</t>
   </si>
   <si>
-    <t>https://cdn-shop.adafruit.com/product-files/2686/SK6812MINI_REV.01-1-2.pdf</t>
+    <t>https://cdn-shop.adafruit.com/product-files/4492/Datasheet.pdf</t>
   </si>
   <si>
     <t>3</t>
@@ -307,7 +307,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-31 21:03:40</t>
+    <t>2023-06-01 06:03:09</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@b0111f044335ce82a2366fa9673f79a32cee981a 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
   <si>
     <t>Row</t>
   </si>
@@ -223,12 +223,33 @@
     <t>Conn_02x02_Odd_Even</t>
   </si>
   <si>
-    <t>J1</t>
+    <t>J1 J2</t>
+  </si>
+  <si>
+    <t>middle</t>
   </si>
   <si>
     <t>PinSocket_2x02_P2.00mm_Vertical_SMD</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>R_0201_0603Metric_Pad0.64x0.40mm_HandSolder</t>
+  </si>
+  <si>
     <t>KiBot Bill of Materials</t>
   </si>
   <si>
@@ -268,7 +289,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>25 (25 SMD/ 0 THT)</t>
+    <t>27 (27 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -307,7 +328,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-06-02 11:31:17</t>
+    <t>2023-06-02 13:42:47</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -470,7 +491,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +543,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF0BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8A8A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -621,6 +648,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -654,14 +684,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1073,7 +1103,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1086,7 +1116,7 @@
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
@@ -1095,7 +1125,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1106,55 +1136,55 @@
     </row>
     <row r="2" spans="1:9">
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1162,16 +1192,16 @@
     </row>
     <row r="6" spans="1:9">
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F6" s="3">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1275,18 +1305,47 @@
         <v>27</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="I11" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1302,7 +1361,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -1314,7 +1373,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="39.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="34.7109375" customWidth="1" outlineLevel="1"/>
@@ -1324,7 +1383,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1332,169 +1391,188 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="12">
+        <v>38</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="14">
+        <v>40</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="15">
-        <f>SUM(G10:G12)</f>
+        <v>42</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="16">
+        <f>SUM(G10:G13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="A8" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>50</v>
+      <c r="D9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="19">
         <f>CEILING(BoardQty*12,1)</f>
         <v>12</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="20">
         <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="19">
         <f>CEILING(BoardQty*12,1)</f>
         <v>12</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="20">
         <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="18">
+      <c r="C12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="19">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="G12" s="20">
+        <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G12" s="19">
-        <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
+      <c r="G13" s="20">
+        <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="22" t="s">
-        <v>56</v>
+      <c r="A16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="23" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1515,6 +1593,11 @@
   <conditionalFormatting sqref="E12">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND(ISBLANK(D12),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>AND(ISBLANK(D13),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -1539,72 +1622,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="23" t="s">
-        <v>62</v>
+      <c r="A7" s="24" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="24" t="s">
-        <v>63</v>
+      <c r="A8" s="25" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="25" t="s">
-        <v>64</v>
+      <c r="A9" s="26" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="26" t="s">
-        <v>65</v>
+      <c r="A10" s="27" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="27" t="s">
-        <v>66</v>
+      <c r="A11" s="28" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="28" t="s">
-        <v>67</v>
+      <c r="A12" s="29" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="29" t="s">
-        <v>68</v>
+      <c r="A13" s="30" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="30" t="s">
-        <v>69</v>
+      <c r="A14" s="31" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="31" t="s">
-        <v>70</v>
+      <c r="A15" s="32" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@f5a3a7607b83ba6a9be8e167990e6122bdc46594 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -8,13 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
-    <sheet name="Costs" sheetId="2" r:id="rId2"/>
-    <sheet name="Colors" sheetId="3" r:id="rId3"/>
+    <sheet name="DNF" sheetId="2" r:id="rId2"/>
+    <sheet name="Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="Costs (DNF)" sheetId="4" r:id="rId4"/>
+    <sheet name="Colors" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="1">'Costs'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="2">'Costs'!$G$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="1">'Costs'!$G$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
+    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="2">'Costs'!$G$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -139,8 +144,127 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use the minimum extend price across distributors not taking account available quantities.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schematic identifier for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PCB footprint for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Manufacturer number for each part and link to it's datasheet (Ctrl-click).
+Purple -&gt; Obsolete part detected by one of the distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of each part needed.
+Gray -&gt; No manf# provided.
+Red -&gt; No parts available.
+Orange -&gt; Not enough parts available.
+Yellow -&gt; Parts available, but haven't purchased enough.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum unit price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum extended price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="86">
   <si>
     <t>Row</t>
   </si>
@@ -169,6 +293,9 @@
     <t>Datasheet</t>
   </si>
   <si>
+    <t>Supplier</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -193,7 +320,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>~</t>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Samsung%20PDFs/CL_Series_MLCC_ds.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/samsung-electro-mechanics/CL03A105MQ3CSNH/3894097</t>
   </si>
   <si>
     <t>2</t>
@@ -214,9 +344,87 @@
     <t>https://cdn-shop.adafruit.com/product-files/4492/Datasheet.pdf</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/4492/11569136</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>R_0201_0603Metric_Pad0.64x0.40mm_HandSolder</t>
+  </si>
+  <si>
+    <t>https://api.pim.na.industrial.panasonic.com/file_stream/main/fileversion/1242</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/panasonic-electronic-components/ERJ-1GNJ331C/2035775</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-led-ring</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-05-29</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>7.0.5.1-1-g8f565ef7f0-dirty-deb11</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>27 (27 SMD/ 0 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>25 (25 SMD/ 0 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
     <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -232,73 +440,13 @@
     <t>PinSocket_2x02_P2.00mm_Vertical_SMD</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>R_0201_0603Metric_Pad0.64x0.40mm_HandSolder</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-led-ring</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-05-29</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>7.0.5.1-1-g8f565ef7f0-dirty-deb11</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>27 (27 SMD/ 0 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>https://gct.co/files/drawings/bf100.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/gct/BF100-04-A-D-1-0640-L-C/16396866</t>
   </si>
   <si>
     <t>Global Part Info</t>
@@ -328,7 +476,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-06-03 10:48:42</t>
+    <t>2023-06-03 11:29:05</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -491,7 +639,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,12 +672,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF0FFF4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -548,7 +690,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8A8A"/>
+        <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -645,53 +787,50 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -776,8 +915,112 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1464384</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2378784</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>921459</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1103,7 +1346,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1113,19 +1356,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="10" max="10" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" customHeight="1">
+    <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1133,55 +1377,56 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="C4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="C4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>51</v>
@@ -1190,21 +1435,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="F6" s="3">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1232,126 +1477,109 @@
       <c r="I8" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="8" t="s">
+      <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="45" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="11" t="s">
+      <c r="I11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="J11" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -1361,7 +1589,186 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="44.7109375" customWidth="1"/>
+    <col min="10" max="10" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="32" customHeight="1">
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -1375,7 +1782,7 @@
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="39.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="34.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
@@ -1383,7 +1790,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1391,188 +1798,175 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="13">
+      <c r="F2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="15">
+      <c r="F3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="13">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="16">
-        <f>SUM(G10:G13)</f>
+      <c r="F4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="14">
+        <f>SUM(G10:G12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="A8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="19" t="s">
+      <c r="D9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1">
+      <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="19">
+      <c r="C10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="17">
         <f>CEILING(BoardQty*12,1)</f>
         <v>12</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="18">
         <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1">
-      <c r="A11" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="19" t="s">
+      <c r="A11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="19">
+      <c r="C11" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="17">
         <f>CEILING(BoardQty*12,1)</f>
         <v>12</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="18">
         <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
-      </c>
-      <c r="G12" s="20">
+    <row r="12" spans="1:7" ht="30" customHeight="1">
+      <c r="A12" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="17">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="18">
         <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="20">
-        <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
-        <v/>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="23" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1595,13 +1989,187 @@
       <formula>AND(ISBLANK(D12),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>AND(ISBLANK(D13),TRUE())</formula>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId2"/>
+    <hyperlink ref="D12" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="34.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="32" customHeight="1">
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="13">
+        <f>TotalCost/BoardQty</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="14">
+        <f>SUM(G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="17">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="18">
+        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="D1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(ISBLANK(D10),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D10" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -1609,7 +2177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1622,72 +2190,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="8" t="s">
-        <v>67</v>
+      <c r="A4" s="22" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="24" t="s">
-        <v>69</v>
+      <c r="A7" s="23" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="25" t="s">
-        <v>70</v>
+      <c r="A8" s="24" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="26" t="s">
-        <v>71</v>
+      <c r="A9" s="25" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="27" t="s">
-        <v>72</v>
+      <c r="A10" s="26" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="28" t="s">
-        <v>73</v>
+      <c r="A11" s="27" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="29" t="s">
-        <v>74</v>
+      <c r="A12" s="28" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="30" t="s">
-        <v>75</v>
+      <c r="A13" s="29" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="31" t="s">
-        <v>76</v>
+      <c r="A14" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="32" t="s">
-        <v>77</v>
+      <c r="A15" s="31" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@a35f995714e23c109d5ac7ae7a3b983694484859 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
   <si>
     <t>Row</t>
   </si>
@@ -338,6 +338,9 @@
     <t>D1 D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12</t>
   </si>
   <si>
+    <t>SK6812_EC15</t>
+  </si>
+  <si>
     <t>LED_SK6812_EC15_1.5x1.5mm</t>
   </si>
   <si>
@@ -476,7 +479,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-06-03 11:40:53</t>
+    <t>2023-06-03 12:20:12</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -1369,7 +1372,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1381,13 +1384,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3">
         <v>4</v>
@@ -1395,41 +1398,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1437,13 +1440,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F6" s="3">
         <v>25</v>
@@ -1527,10 +1530,10 @@
         <v>23</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>16</v>
@@ -1539,30 +1542,30 @@
         <v>17</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>10</v>
@@ -1571,10 +1574,10 @@
         <v>17</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1612,7 +1615,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1624,13 +1627,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3">
         <v>4</v>
@@ -1638,41 +1641,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1680,13 +1683,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F6" s="3">
         <v>25</v>
@@ -1729,31 +1732,31 @@
         <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1780,7 +1783,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="34.7109375" customWidth="1" outlineLevel="1"/>
@@ -1790,7 +1793,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1798,13 +1801,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G2" s="11">
         <v>1</v>
@@ -1812,13 +1815,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G3" s="13">
         <f>TotalCost/BoardQty</f>
@@ -1827,13 +1830,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G4" s="14">
         <f>SUM(G10:G12)</f>
@@ -1842,23 +1845,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -1878,16 +1881,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -1917,13 +1920,13 @@
         <v>23</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="17">
         <f>CEILING(BoardQty*12,1)</f>
@@ -1936,16 +1939,16 @@
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E12" s="17">
         <f>BoardQty*1</f>
@@ -1958,15 +1961,15 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2023,7 +2026,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2031,13 +2034,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G2" s="11">
         <v>1</v>
@@ -2045,13 +2048,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G3" s="13">
         <f>TotalCost/BoardQty</f>
@@ -2060,13 +2063,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G4" s="14">
         <f>SUM(G10)</f>
@@ -2075,23 +2078,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -2111,30 +2114,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E10" s="17">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2147,15 +2150,15 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2190,72 +2193,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@12c7b2ffcd00eb9e26b7f3a3736545f789e05617 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -332,7 +332,7 @@
     <t>RGB LED with integrated controller</t>
   </si>
   <si>
-    <t>SK6812MINI</t>
+    <t>SK6812</t>
   </si>
   <si>
     <t>D1 D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12</t>
@@ -344,7 +344,7 @@
     <t>LED_SK6812_EC15_1.5x1.5mm</t>
   </si>
   <si>
-    <t>https://cdn-shop.adafruit.com/product-files/4492/Datasheet.pdf</t>
+    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/4492/11569136</t>
@@ -479,7 +479,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-06-03 20:06:21</t>
+    <t>2023-06-03 21:31:22</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@0806d0484308088faf02c68ed3784f717a60aba5 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="102">
   <si>
     <t>Row</t>
   </si>
@@ -296,6 +296,12 @@
     <t>Supplier</t>
   </si>
   <si>
+    <t>Sim.Device</t>
+  </si>
+  <si>
+    <t>Sim.Pins</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -326,6 +332,9 @@
     <t>https://www.digikey.ch/en/products/detail/samsung-electro-mechanics/CL03A105MQ3CSNH/3894097</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -359,15 +368,30 @@
     <t>R</t>
   </si>
   <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>R_0201_0603Metric_Pad0.64x0.40mm_HandSolder</t>
+  </si>
+  <si>
+    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/RDA0000/AOA0000C301.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/panasonic-electronic-components/ERJ-1GN0R00C/3982613</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
     <t>330</t>
   </si>
   <si>
-    <t>R_0201_0603Metric_Pad0.64x0.40mm_HandSolder</t>
-  </si>
-  <si>
     <t>https://api.pim.na.industrial.panasonic.com/file_stream/main/fileversion/1242</t>
   </si>
   <si>
@@ -413,13 +437,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>27 (27 SMD/ 0 THT)</t>
+    <t>29 (29 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>25 (25 SMD/ 0 THT)</t>
+    <t>26 (26 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -428,6 +452,30 @@
     <t>Total Components:</t>
   </si>
   <si>
+    <t>75V 0.15A Fast Switching Diode, SOD-123</t>
+  </si>
+  <si>
+    <t>1N4148W</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D_SOD-923</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/NSR05T40P2T5G/5761753</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>1=K 2=A</t>
+  </si>
+  <si>
     <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -443,9 +491,6 @@
     <t>PinSocket_2x02_P2.00mm_Vertical_SMD</t>
   </si>
   <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
     <t>https://gct.co/files/drawings/bf100.pdf</t>
   </si>
   <si>
@@ -479,7 +524,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-06-05 16:14:13</t>
+    <t>2023-06-20 15:22:48</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -642,7 +687,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -675,6 +720,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF8080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF0FFF4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -693,7 +744,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
+        <fgColor rgb="FFFF8A8A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -788,6 +839,12 @@
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -823,17 +880,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1023,7 +1077,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>921459</xdr:colOff>
+      <xdr:colOff>950034</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1349,7 +1403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1368,11 +1422,13 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" customHeight="1">
+    <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1381,78 +1437,80 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="C3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="C3" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="C4" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="C4" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="C5" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="C5" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F6" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1483,106 +1541,168 @@
       <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1">
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="I11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="L11" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="C12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>35</v>
+      <c r="D12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -1592,7 +1712,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1611,11 +1731,13 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="44.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" customHeight="1">
+    <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1624,78 +1746,80 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="C3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="C3" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="C4" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="C4" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="C5" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="C5" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F6" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1726,42 +1850,92 @@
       <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="45" customHeight="1">
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>61</v>
+        <v>67</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -1771,7 +1945,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -1793,7 +1967,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1801,175 +1975,197 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="11">
+        <v>46</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="13">
+        <v>48</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="14">
-        <f>SUM(G10:G12)</f>
+        <v>50</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="16">
+        <f>SUM(G10:G13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="A8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>66</v>
+      <c r="D9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
-      <c r="A10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="17">
+      <c r="B10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="19">
         <f>CEILING(BoardQty*12,1)</f>
         <v>12</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="20">
         <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1">
-      <c r="A11" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="17" t="s">
+      <c r="A11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="17">
+      <c r="B11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="19">
         <f>CEILING(BoardQty*12,1)</f>
         <v>12</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="20">
         <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1">
-      <c r="A12" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="17">
+      <c r="B12" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="20">
         <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>71</v>
+    <row r="13" spans="1:7" ht="30" customHeight="1">
+      <c r="A13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="20">
+        <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="21" t="s">
-        <v>72</v>
+        <v>85</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="23" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1992,20 +2188,26 @@
       <formula>AND(ISBLANK(D12),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>AND(ISBLANK(D13),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
     <hyperlink ref="D12" r:id="rId3"/>
+    <hyperlink ref="D13" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -2017,6 +2219,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="40.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="34.7109375" customWidth="1" outlineLevel="1"/>
@@ -2026,7 +2229,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2034,131 +2237,150 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="11">
+        <v>46</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="13">
+        <v>48</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="14">
-        <f>SUM(G10)</f>
+        <v>50</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="16">
+        <f>SUM(G10:G11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="A8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="16" t="s">
+      <c r="C10" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="17">
+      <c r="E10" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="20">
+        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G10" s="18">
-        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+      <c r="G11" s="20">
+        <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
         <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="21" t="s">
-        <v>72</v>
+        <v>85</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="23" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2171,8 +2393,13 @@
       <formula>AND(ISBLANK(D10),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND(ISBLANK(D11),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -2193,72 +2420,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="22" t="s">
-        <v>76</v>
+      <c r="A4" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="23" t="s">
-        <v>78</v>
+      <c r="A7" s="24" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="24" t="s">
-        <v>79</v>
+      <c r="A8" s="25" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="25" t="s">
-        <v>80</v>
+      <c r="A9" s="26" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="26" t="s">
-        <v>81</v>
+      <c r="A10" s="27" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="27" t="s">
-        <v>82</v>
+      <c r="A11" s="28" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="28" t="s">
-        <v>83</v>
+      <c r="A12" s="29" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="29" t="s">
-        <v>84</v>
+      <c r="A13" s="30" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="30" t="s">
-        <v>85</v>
+      <c r="A14" s="31" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="31" t="s">
-        <v>86</v>
+      <c r="A15" s="32" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-led-ring@ae99860ab7014f392fbd04294ef362df9307f88a 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-led-ring-bom.xlsx
+++ b/BoM/Costs/pedalboard-led-ring-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="105">
   <si>
     <t>Row</t>
   </si>
@@ -353,7 +353,7 @@
     <t>LED_SK6812_EC15_1.5x1.5mm</t>
   </si>
   <si>
-    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
+    <t>http://www.normandled.com/upload/202112/SK9810-EC15%20LED%20Datasheet.pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/4492/11569136</t>
@@ -362,6 +362,30 @@
     <t>3</t>
   </si>
   <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>PinSocket_2x02_P2.00mm_Vertical_SMD</t>
+  </si>
+  <si>
+    <t>https://gct.co/files/drawings/bf100.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/gct/BF100-04-A-D-1-0640-L-C/16396866</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -383,7 +407,7 @@
     <t>https://www.digikey.ch/en/products/detail/panasonic-electronic-components/ERJ-1GN0R00C/3982613</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
   </si>
   <si>
     <t>R1</t>
@@ -443,7 +467,7 @@
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>26 (26 SMD/ 0 THT)</t>
+    <t>27 (27 SMD/ 0 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -476,27 +500,12 @@
     <t>1=K 2=A</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J1 J2</t>
+    <t>J1</t>
   </si>
   <si>
     <t>middle</t>
   </si>
   <si>
-    <t>PinSocket_2x02_P2.00mm_Vertical_SMD</t>
-  </si>
-  <si>
-    <t>https://gct.co/files/drawings/bf100.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/en/products/detail/gct/BF100-04-A-D-1-0640-L-C/16396866</t>
-  </si>
-  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -524,10 +533,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-06-20 15:28:54</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
+    <t>2023-07-22 11:30:11</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>
@@ -1403,7 +1412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1413,8 +1422,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" customWidth="1"/>
@@ -1428,7 +1437,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1442,55 +1451,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1498,16 +1507,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F6" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1624,7 +1633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1">
+    <row r="11" spans="1:12" ht="45" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1667,19 +1676,19 @@
         <v>39</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>12</v>
@@ -1688,15 +1697,53 @@
         <v>19</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>22</v>
       </c>
       <c r="L12" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1737,7 +1784,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1751,55 +1798,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1807,16 +1854,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F6" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1862,37 +1909,37 @@
         <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" customHeight="1">
@@ -1900,31 +1947,31 @@
         <v>23</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="I10" s="11" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>22</v>
@@ -1945,7 +1992,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -1967,7 +2014,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1975,13 +2022,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -1989,13 +2036,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2004,38 +2051,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G13)</f>
+        <f>SUM(G10:G14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2055,16 +2102,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -2111,7 +2158,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1">
+    <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
@@ -2135,16 +2182,16 @@
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -2155,17 +2202,39 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="23" t="s">
-        <v>87</v>
+    <row r="14" spans="1:7" ht="30" customHeight="1">
+      <c r="A14" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="20">
+        <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2193,15 +2262,21 @@
       <formula>AND(ISBLANK(D13),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>AND(ISBLANK(D14),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
     <hyperlink ref="D12" r:id="rId3"/>
     <hyperlink ref="D13" r:id="rId4"/>
+    <hyperlink ref="D14" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -2229,7 +2304,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2237,13 +2312,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2251,13 +2326,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2266,13 +2341,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G11)</f>
@@ -2281,23 +2356,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2317,27 +2392,27 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E10" s="19">
         <f>BoardQty*1</f>
@@ -2350,20 +2425,20 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="E11" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G11" s="20">
         <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
@@ -2372,15 +2447,15 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="21" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="23" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2420,72 +2495,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>